<commit_message>
Excel: added super simple expression support to filters for string matching.
</commit_message>
<xml_diff>
--- a/Archivist/src/test/resources/excelFile.xlsx
+++ b/Archivist/src/test/resources/excelFile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Table 1</t>
   </si>
@@ -21,6 +21,9 @@
   </si>
   <si>
     <t>One</t>
+  </si>
+  <si>
+    <t>beer_kettle_01.jpg</t>
   </si>
   <si>
     <t>B</t>
@@ -267,10 +270,10 @@
     <xf numFmtId="59" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1451,18 +1454,20 @@
       <c r="F4" s="13">
         <v>40877</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" t="s" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" t="s" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="11">
         <v>2</v>
       </c>
       <c r="D5" t="s" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="11">
         <v>1.3</v>
@@ -1470,18 +1475,20 @@
       <c r="F5" s="13">
         <v>40878</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" t="s" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" ht="20.35" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" t="s" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="11">
         <v>3</v>
       </c>
       <c r="D6" t="s" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="11">
         <v>1.4</v>
@@ -1489,18 +1496,20 @@
       <c r="F6" s="13">
         <v>40879</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" t="s" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" ht="20.35" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" t="s" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="11">
         <v>4</v>
       </c>
       <c r="D7" t="s" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="11">
         <v>1.5</v>
@@ -1508,18 +1517,20 @@
       <c r="F7" s="13">
         <v>40880</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" t="s" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" t="s" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="11">
         <v>5</v>
       </c>
       <c r="D8" t="s" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="11">
         <v>2.1</v>
@@ -1527,18 +1538,20 @@
       <c r="F8" s="13">
         <v>40881</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" t="s" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" t="s" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="11">
         <v>6</v>
       </c>
       <c r="D9" t="s" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="11">
         <v>2.2</v>
@@ -1546,18 +1559,20 @@
       <c r="F9" s="13">
         <v>40882</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" t="s" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" ht="20.35" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" t="s" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="11">
         <v>7</v>
       </c>
       <c r="D10" t="s" s="12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" s="11">
         <v>2.3</v>
@@ -1565,124 +1580,126 @@
       <c r="F10" s="13">
         <v>40883</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="G10" t="s" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" ht="20.35" customHeight="1">
       <c r="A11" s="9"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="A12" s="9"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" s="9"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" s="9"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
       <c r="A15" s="9"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
       <c r="A16" s="9"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
       <c r="A17" s="9"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
       <c r="A18" s="9"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
       <c r="A19" s="9"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
       <c r="A20" s="9"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" ht="20.35" customHeight="1">
       <c r="A21" s="9"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
       <c r="A22" s="9"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
       <c r="A23" s="9"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="14"/>
+      <c r="G23" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Excel: adding support for dropping data into keywords, confidence level=1
</commit_message>
<xml_diff>
--- a/Archivist/src/test/resources/excelFile.xlsx
+++ b/Archivist/src/test/resources/excelFile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Table 1</t>
   </si>
@@ -20,7 +20,7 @@
     <t>A</t>
   </si>
   <si>
-    <t>One</t>
+    <t>One,Ten</t>
   </si>
   <si>
     <t>beer_kettle_01.jpg</t>
@@ -32,34 +32,52 @@
     <t>Two</t>
   </si>
   <si>
+    <t>beer_kettle_02.jpg</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
     <t>Three</t>
   </si>
   <si>
+    <t>beer_kettle_03.jpg</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
     <t>Four</t>
   </si>
   <si>
+    <t>beer_kettle_04.jpg</t>
+  </si>
+  <si>
     <t>E</t>
   </si>
   <si>
     <t>Five</t>
   </si>
   <si>
+    <t>beer_kettle_05.jpg</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
     <t>Six</t>
   </si>
   <si>
+    <t>beer_kettle_06.jpg</t>
+  </si>
+  <si>
     <t>G</t>
   </si>
   <si>
     <t>Seven</t>
+  </si>
+  <si>
+    <t>beer_kettle_07.jpg</t>
   </si>
 </sst>
 </file>
@@ -1476,19 +1494,19 @@
         <v>40878</v>
       </c>
       <c r="G5" t="s" s="12">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" ht="20.35" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" t="s" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="11">
         <v>3</v>
       </c>
       <c r="D6" t="s" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="11">
         <v>1.4</v>
@@ -1497,19 +1515,19 @@
         <v>40879</v>
       </c>
       <c r="G6" t="s" s="12">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" ht="20.35" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" t="s" s="10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="11">
         <v>4</v>
       </c>
       <c r="D7" t="s" s="12">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E7" s="11">
         <v>1.5</v>
@@ -1518,19 +1536,19 @@
         <v>40880</v>
       </c>
       <c r="G7" t="s" s="12">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" t="s" s="10">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C8" s="11">
         <v>5</v>
       </c>
       <c r="D8" t="s" s="12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E8" s="11">
         <v>2.1</v>
@@ -1539,19 +1557,19 @@
         <v>40881</v>
       </c>
       <c r="G8" t="s" s="12">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" t="s" s="10">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="11">
         <v>6</v>
       </c>
       <c r="D9" t="s" s="12">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E9" s="11">
         <v>2.2</v>
@@ -1560,19 +1578,19 @@
         <v>40882</v>
       </c>
       <c r="G9" t="s" s="12">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" ht="20.35" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" t="s" s="10">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="11">
         <v>7</v>
       </c>
       <c r="D10" t="s" s="12">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E10" s="11">
         <v>2.3</v>
@@ -1581,7 +1599,7 @@
         <v>40883</v>
       </c>
       <c r="G10" t="s" s="12">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" ht="20.35" customHeight="1">

</xml_diff>